<commit_message>
All updates for GUI
</commit_message>
<xml_diff>
--- a/tests/link_budget_validation.xlsx
+++ b/tests/link_budget_validation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\GitHub\pysim5g_application\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoangNam\Documents\GitHub\pysim5g_application\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87049AE-0F40-4497-AC7D-AF4A29286189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5500944-AE5A-4EA3-82EC-2CE1FDEE64F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="link_buget_example 1" sheetId="1" r:id="rId1"/>
-    <sheet name="4G-5G CM LUT" sheetId="2" r:id="rId2"/>
-    <sheet name="Energy_consumption" sheetId="3" r:id="rId3"/>
+    <sheet name="Giá trị kiểm thử link budget" sheetId="1" r:id="rId1"/>
+    <sheet name="Bảng tra SE 4G và 5G" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
   <si>
     <t>Tx Gain (dBi)</t>
   </si>
@@ -120,12 +119,6 @@
     <t>CQI index</t>
   </si>
   <si>
-    <t>4G LTE (Zarrinkoub, 2014)</t>
-  </si>
-  <si>
-    <t>5G (ETSI, 2018)</t>
-  </si>
-  <si>
     <t>Modulation</t>
   </si>
   <si>
@@ -145,6 +138,51 @@
   </si>
   <si>
     <t>256QAM</t>
+  </si>
+  <si>
+    <t>Area (km^2)</t>
+  </si>
+  <si>
+    <t>Capacity (Mbps)</t>
+  </si>
+  <si>
+    <t>Capacity (bps/km2)</t>
+  </si>
+  <si>
+    <t>Capacity (Mbps/km2)</t>
+  </si>
+  <si>
+    <t>Tính I + N</t>
+  </si>
+  <si>
+    <t>Tính SINR</t>
+  </si>
+  <si>
+    <t>Hiệu suất phổ SE</t>
+  </si>
+  <si>
+    <t>Tính nhiễu (N)</t>
+  </si>
+  <si>
+    <t>Tính công suất thu (received power)</t>
+  </si>
+  <si>
+    <t>Tính can nhiễu (Interference)</t>
+  </si>
+  <si>
+    <t>Rx Power (dBm)</t>
+  </si>
+  <si>
+    <t>Tx Power (dBm)</t>
+  </si>
+  <si>
+    <t>Area Capacity</t>
+  </si>
+  <si>
+    <t>1x1 (4G), 8x8 (5G)</t>
+  </si>
+  <si>
+    <t>Transmission Type</t>
   </si>
   <si>
     <r>
@@ -157,7 +195,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>Understanding LTE with MATLAB: From Mathematical Modeling to Simulation and Prototyping</t>
     </r>
@@ -167,88 +204,38 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>. John Wiley &amp; Sons.</t>
     </r>
   </si>
   <si>
-    <t>ETSI. 2018. ‘5G; NR; Physical Layer Procedures for Data (3GPP TS 38.214 Version 15.3.0 Release 15)’. Valbonne, France: ETSI.</t>
-  </si>
-  <si>
-    <t>Energy consumption</t>
-  </si>
-  <si>
-    <t>Power (dBm)</t>
-  </si>
-  <si>
-    <t>Power linear (watts)</t>
-  </si>
-  <si>
-    <t>Power per site (watts)</t>
-  </si>
-  <si>
-    <t>Total power per area (watts)</t>
-  </si>
-  <si>
-    <t>Throughput per area (bps per km^2)</t>
-  </si>
-  <si>
-    <t>Energy efficiency (bps/watt)</t>
-  </si>
-  <si>
-    <t>Cells per site (watts)</t>
-  </si>
-  <si>
-    <t>Sites per area</t>
-  </si>
-  <si>
-    <t>Area (km^2)</t>
-  </si>
-  <si>
-    <t>Capacity (Mbps)</t>
-  </si>
-  <si>
-    <t>Capacity (bps/km2)</t>
-  </si>
-  <si>
-    <t>Capacity (Mbps/km2)</t>
-  </si>
-  <si>
-    <t>Tính công suất thu</t>
-  </si>
-  <si>
-    <t>CS thu Rx (dBm)</t>
-  </si>
-  <si>
-    <t>CS phát Tx (dBm)</t>
-  </si>
-  <si>
-    <t>Tính I + N</t>
-  </si>
-  <si>
-    <t>Tính interference I</t>
-  </si>
-  <si>
-    <t>Tính nhiễu (noise) N</t>
-  </si>
-  <si>
-    <t>Tính SINR</t>
-  </si>
-  <si>
-    <t>Hiệu suất phổ SE</t>
+    <t>4G LTE</t>
+  </si>
+  <si>
+    <t>5G NR</t>
+  </si>
+  <si>
+    <t>*SE được tra theo kết quả mapping SINR và Efficiency</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>"Bảng tra SE 4G và 5G" - tham khảo từ chuẩn 3GPP TS 38.214</t>
+  </si>
+  <si>
+    <t>3GPP TS 38.214 V17.2.0; NR; Physical layer procedures for data (Release 17).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -307,19 +294,45 @@
       <family val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,7 +343,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -429,63 +442,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -494,7 +475,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -509,13 +490,69 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -524,12 +561,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -539,36 +574,80 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -633,91 +712,93 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1032,31 +1113,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="4" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="8" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="8" width="15.85546875" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="1025" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -1106,7 +1190,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1115,55 +1199,55 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
+      <c r="A9" s="5">
         <f>(B9+C9-D9)-E9-F9+G9-H9</f>
         <v>-73</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="6">
         <v>40</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="6">
         <v>16</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="6">
         <v>124</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="6">
         <v>4</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="6">
         <v>4</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1180,55 +1264,55 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="25" t="s">
+      <c r="A11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="5">
         <f>(B12+C12-D12)-E12-F12+G12-H12</f>
         <v>-62</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="6">
         <v>40</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="6">
         <v>16</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="6">
         <v>1</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="6">
         <v>113</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="6">
         <v>4</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="6">
         <v>4</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1246,10 +1330,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>0</v>
@@ -1309,7 +1393,7 @@
     </row>
     <row r="18" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1363,7 +1447,7 @@
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,7 +1483,7 @@
     </row>
     <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1429,7 +1513,7 @@
     </row>
     <row r="33" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,15 +1523,21 @@
       <c r="B34" s="20" t="s">
         <v>11</v>
       </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
-        <v>1.4765999999999999</v>
+        <v>8</v>
       </c>
       <c r="B35" s="16">
         <f>A30</f>
         <v>2.3010299956596381</v>
       </c>
+      <c r="C35" s="42" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1464,20 +1554,20 @@
       <c r="C38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="39" t="s">
-        <v>47</v>
+      <c r="D38" s="29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="23">
         <f>B39*C39</f>
-        <v>14766000</v>
-      </c>
-      <c r="B39" s="30">
+        <v>80000000</v>
+      </c>
+      <c r="B39" s="24">
         <f>A35</f>
-        <v>1.4765999999999999</v>
-      </c>
-      <c r="C39" s="43">
+        <v>8</v>
+      </c>
+      <c r="C39" s="30">
         <f>10000000</f>
         <v>10000000</v>
       </c>
@@ -1487,24 +1577,24 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
-        <v>48</v>
+      <c r="A41" s="31" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="45">
+      <c r="A42" s="32">
         <f>A39/1000000</f>
-        <v>14.766</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B45" s="22" t="s">
         <v>13</v>
@@ -1512,20 +1602,20 @@
       <c r="C45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="39" t="s">
-        <v>47</v>
+      <c r="D45" s="29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="23">
         <f>B46*C46/D46</f>
-        <v>68201248.647267997</v>
-      </c>
-      <c r="B46" s="30">
+        <v>369504259.22940809</v>
+      </c>
+      <c r="B46" s="24">
         <f>A35</f>
-        <v>1.4765999999999999</v>
-      </c>
-      <c r="C46" s="43">
+        <v>8</v>
+      </c>
+      <c r="C46" s="30">
         <f>E20</f>
         <v>10000000</v>
       </c>
@@ -1535,17 +1625,20 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
-        <v>50</v>
+      <c r="A48" s="31" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="45">
+      <c r="A49" s="32">
         <f>A46/1000000</f>
-        <v>68.201248647268002</v>
+        <v>369.50425922940809</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C35" location="'Bảng tra SE 4G và 5G'!H7" display="&quot;Bảng tra SE 4G và 5G&quot; - tham khảo từ chuẩn 3GPP TS 38.214" xr:uid="{00595A85-12AA-4685-8521-52DFD13E61C5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1553,15 +1646,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638A3F84-9186-47E2-B75B-D0A8861F43CA}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
@@ -1570,544 +1664,508 @@
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="C1" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="51"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="44"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49" t="s">
+      <c r="D2" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50" t="s">
+      <c r="E2" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="38">
+        <v>1</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="38">
+        <v>78</v>
+      </c>
+      <c r="E3" s="38">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="38">
+        <v>78</v>
+      </c>
+      <c r="H3" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="I3" s="39">
+        <v>-6.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="25">
+        <v>2</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="25">
+        <v>120</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0.2344</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="25">
+        <v>193</v>
+      </c>
+      <c r="H4" s="25">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I4" s="26">
+        <v>-4.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="25">
+        <v>3</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="25">
+        <v>193</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0.377</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="25">
+        <v>449</v>
+      </c>
+      <c r="H5" s="25">
+        <v>4.42</v>
+      </c>
+      <c r="I5" s="26">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="25">
+        <v>4</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="25">
+        <v>308</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0.60160000000000002</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="25">
+        <v>378</v>
+      </c>
+      <c r="H6" s="25">
+        <v>6.4</v>
+      </c>
+      <c r="I6" s="26">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="25">
+        <v>5</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="25">
+        <v>449</v>
+      </c>
+      <c r="E7" s="25">
+        <v>0.877</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="25">
+        <v>490</v>
+      </c>
+      <c r="H7" s="25">
+        <v>8</v>
+      </c>
+      <c r="I7" s="26">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="25">
+        <v>6</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="25">
+        <v>602</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1.1758</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="25">
+        <v>616</v>
+      </c>
+      <c r="H8" s="25">
+        <v>10.82</v>
+      </c>
+      <c r="I8" s="26">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="25">
+        <v>7</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="25">
+        <v>378</v>
+      </c>
+      <c r="E9" s="25">
+        <v>1.4765999999999999</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="25">
+        <v>466</v>
+      </c>
+      <c r="H9" s="25">
+        <v>12.4</v>
+      </c>
+      <c r="I9" s="26">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="25">
+        <v>8</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="25">
+        <v>490</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1.9140999999999999</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="25">
+        <v>567</v>
+      </c>
+      <c r="H10" s="25">
+        <v>16</v>
+      </c>
+      <c r="I10" s="26">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="25">
+        <v>9</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="25">
+        <v>616</v>
+      </c>
+      <c r="E11" s="25">
+        <v>2.4062999999999999</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="25">
+        <v>666</v>
+      </c>
+      <c r="H11" s="25">
+        <v>19</v>
+      </c>
+      <c r="I11" s="26">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="25">
+        <v>10</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="25">
+        <v>466</v>
+      </c>
+      <c r="E12" s="25">
+        <v>2.7305000000000001</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="25">
+        <v>772</v>
+      </c>
+      <c r="H12" s="25">
+        <v>22</v>
+      </c>
+      <c r="I12" s="26">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="25">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="51"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
-        <v>1</v>
-      </c>
-      <c r="B3" s="32" t="s">
+      <c r="C13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="32">
-        <v>7.6200000000000004E-2</v>
-      </c>
-      <c r="D3" s="32">
-        <v>0.15229999999999999</v>
-      </c>
-      <c r="E3" s="32" t="s">
+      <c r="D13" s="25">
+        <v>567</v>
+      </c>
+      <c r="E13" s="25">
+        <v>3.3222999999999998</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="32">
-        <v>78</v>
-      </c>
-      <c r="G3" s="32">
-        <v>0.15229999999999999</v>
-      </c>
-      <c r="H3" s="34">
-        <v>-6.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
-        <v>2</v>
-      </c>
-      <c r="B4" s="32" t="s">
+      <c r="G13" s="25">
+        <v>873</v>
+      </c>
+      <c r="H13" s="25">
+        <v>28</v>
+      </c>
+      <c r="I13" s="26">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="25">
+        <v>12</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="32">
-        <v>0.1172</v>
-      </c>
-      <c r="D4" s="32">
-        <v>0.2344</v>
-      </c>
-      <c r="E4" s="32" t="s">
+      <c r="D14" s="25">
+        <v>666</v>
+      </c>
+      <c r="E14" s="25">
+        <v>3.9022999999999999</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="25">
+        <v>711</v>
+      </c>
+      <c r="H14" s="25">
         <v>32</v>
       </c>
-      <c r="F4" s="32">
-        <v>193</v>
-      </c>
-      <c r="G4" s="32">
-        <v>0.377</v>
-      </c>
-      <c r="H4" s="34">
-        <v>-4.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
-        <v>3</v>
-      </c>
-      <c r="B5" s="32" t="s">
+      <c r="I14" s="26">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="25">
+        <v>13</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="32">
-        <v>0.1885</v>
-      </c>
-      <c r="D5" s="32">
-        <v>0.377</v>
-      </c>
-      <c r="E5" s="32" t="s">
+      <c r="D15" s="25">
+        <v>772</v>
+      </c>
+      <c r="E15" s="25">
+        <v>4.5233999999999996</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="25">
+        <v>797</v>
+      </c>
+      <c r="H15" s="25">
+        <v>38</v>
+      </c>
+      <c r="I15" s="26">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="25">
+        <v>14</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="32">
-        <v>449</v>
-      </c>
-      <c r="G5" s="32">
-        <v>0.877</v>
-      </c>
-      <c r="H5" s="34">
-        <v>-2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
-        <v>4</v>
-      </c>
-      <c r="B6" s="32" t="s">
+      <c r="D16" s="25">
+        <v>873</v>
+      </c>
+      <c r="E16" s="25">
+        <v>5.1151999999999997</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="25">
+        <v>885</v>
+      </c>
+      <c r="H16" s="25">
+        <v>44</v>
+      </c>
+      <c r="I16" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="27">
+        <v>15</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="32">
-        <v>308</v>
-      </c>
-      <c r="D6" s="32">
-        <v>0.60160000000000002</v>
-      </c>
-      <c r="E6" s="32" t="s">
+      <c r="D17" s="27">
+        <v>948</v>
+      </c>
+      <c r="E17" s="27">
+        <v>5.5547000000000004</v>
+      </c>
+      <c r="F17" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="32">
-        <v>378</v>
-      </c>
-      <c r="G6" s="32">
-        <v>1.4765999999999999</v>
-      </c>
-      <c r="H6" s="34">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
-        <v>5</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="32">
-        <v>449</v>
-      </c>
-      <c r="D7" s="32">
-        <v>0.877</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="32">
-        <v>490</v>
-      </c>
-      <c r="G7" s="32">
-        <v>1.9140999999999999</v>
-      </c>
-      <c r="H7" s="34">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="33">
-        <v>6</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="32">
-        <v>602</v>
-      </c>
-      <c r="D8" s="32">
-        <v>1.1758</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="32">
-        <v>616</v>
-      </c>
-      <c r="G8" s="32">
-        <v>2.4062999999999999</v>
-      </c>
-      <c r="H8" s="34">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
-        <v>7</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="32">
-        <v>378</v>
-      </c>
-      <c r="D9" s="32">
-        <v>1.4765999999999999</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="32">
-        <v>466</v>
-      </c>
-      <c r="G9" s="32">
-        <v>2.7305000000000001</v>
-      </c>
-      <c r="H9" s="34">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="33">
-        <v>8</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="32">
-        <v>490</v>
-      </c>
-      <c r="D10" s="32">
-        <v>1.9140999999999999</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="32">
-        <v>567</v>
-      </c>
-      <c r="G10" s="32">
-        <v>3.3222999999999998</v>
-      </c>
-      <c r="H10" s="34">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
-        <v>9</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="32">
-        <v>616</v>
-      </c>
-      <c r="D11" s="32">
-        <v>2.4062999999999999</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="32">
-        <v>666</v>
-      </c>
-      <c r="G11" s="32">
-        <v>3.9022999999999999</v>
-      </c>
-      <c r="H11" s="34">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
-        <v>10</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="32">
-        <v>466</v>
-      </c>
-      <c r="D12" s="32">
-        <v>2.7305000000000001</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="32">
-        <v>772</v>
-      </c>
-      <c r="G12" s="32">
-        <v>4.5233999999999996</v>
-      </c>
-      <c r="H12" s="34">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
-        <v>11</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="32">
-        <v>567</v>
-      </c>
-      <c r="D13" s="32">
-        <v>3.3222999999999998</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="32">
-        <v>873</v>
-      </c>
-      <c r="G13" s="32">
-        <v>5.1151999999999997</v>
-      </c>
-      <c r="H13" s="34">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="33">
-        <v>12</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="32">
-        <v>666</v>
-      </c>
-      <c r="D14" s="32">
-        <v>3.9022999999999999</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="32">
-        <v>711</v>
-      </c>
-      <c r="G14" s="32">
-        <v>5.5547000000000004</v>
-      </c>
-      <c r="H14" s="34">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
-        <v>13</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="32">
-        <v>772</v>
-      </c>
-      <c r="D15" s="32">
-        <v>4.5233999999999996</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="32">
-        <v>797</v>
-      </c>
-      <c r="G15" s="32">
-        <v>6.2266000000000004</v>
-      </c>
-      <c r="H15" s="34">
-        <v>18.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="33">
-        <v>14</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="32">
-        <v>873</v>
-      </c>
-      <c r="D16" s="32">
-        <v>5.1151999999999997</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="32">
-        <v>885</v>
-      </c>
-      <c r="G16" s="32">
-        <v>6.9141000000000004</v>
-      </c>
-      <c r="H16" s="34">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35">
-        <v>15</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="36">
+      <c r="G17" s="27">
         <v>948</v>
       </c>
-      <c r="D17" s="36">
-        <v>5.5547000000000004</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="36">
-        <v>948</v>
-      </c>
-      <c r="G17" s="36">
-        <v>7.4062999999999999</v>
-      </c>
-      <c r="H17" s="37">
+      <c r="H17" s="27">
+        <v>50</v>
+      </c>
+      <c r="I17" s="28">
         <v>22.7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>37</v>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C36E160-2DE2-4BD6-B8A4-FCF373663928}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40">
-        <v>40</v>
-      </c>
-      <c r="B3" s="6">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40">
-        <f>POWER(10, A3/10)/1000</f>
-        <v>10</v>
-      </c>
-      <c r="B6" s="6">
-        <f>A6*B3</f>
-        <v>30</v>
-      </c>
-      <c r="C6" s="7">
-        <f>B6*C3</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40">
-        <v>60000000</v>
-      </c>
-      <c r="B9" s="41">
-        <f>C6/A9</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>